<commit_message>
Adds all IG authors as contact
</commit_message>
<xml_diff>
--- a/output/CodeSystem-Q4MSAnfragekategorie.xlsx
+++ b/output/CodeSystem-Q4MSAnfragekategorie.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-01-21T07:36:48+01:00</t>
+    <t>2022-01-21T07:49:24+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -329,7 +329,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -429,83 +429,99 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>21</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s" s="2">
-        <v>13</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="B18" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="B18" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B21" t="s" s="2">
-        <v>32</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B22" s="2"/>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="2">
         <v>34</v>
       </c>
-      <c r="B23" t="s" s="2">
+      <c r="B25" t="s" s="2">
         <v>35</v>
       </c>
     </row>

</xml_diff>